<commit_message>
Analog WDG and Interrupts
internal MCU temp threshold ( 0 - 100°c)
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="49">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1639,23 +1639,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5">
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" t="s">
-        <v>48</v>
-      </c>
-    </row>
+    <row r="5"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>